<commit_message>
Got all the stuff calculated, trying to get a few more data points
</commit_message>
<xml_diff>
--- a/density.xlsx
+++ b/density.xlsx
@@ -17,18 +17,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve" uniqueCount="4" count="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve" uniqueCount="2" count="2">
   <si>
     <t>set</t>
   </si>
   <si>
-    <t>mass (g)</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -39,10 +33,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A1" sqref="A1:E3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -62,8 +56,8 @@
       <c r="B1" t="str">
         <v>CV (mL)</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
+      <c r="C1" t="str">
+        <v>mass (g)</v>
       </c>
       <c r="D1" t="str">
         <v>density (g/mL)</v>
@@ -73,8 +67,8 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>2</v>
+      <c r="A2" t="str">
+        <v>a</v>
       </c>
       <c r="B2">
         <v>736.76</v>
@@ -92,8 +86,8 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>3</v>
+      <c r="A3" t="str">
+        <v>b</v>
       </c>
       <c r="B3">
         <v>736.76</v>
@@ -108,6 +102,26 @@
       <c r="E3">
         <f>D3*1000</f>
         <v>240.29534719583</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>736.76</v>
+      </c>
+      <c r="C4">
+        <f>193.94-32.8</f>
+        <v>161.14</v>
+      </c>
+      <c r="D4">
+        <f>C4/B4</f>
+        <v>0.218714371029915</v>
+      </c>
+      <c r="E4">
+        <f>D4*1000</f>
+        <v>218.714371029915</v>
       </c>
     </row>
   </sheetData>

</xml_diff>